<commit_message>
Updated Leave 1/23/2024 4:21 pm
</commit_message>
<xml_diff>
--- a/NEW HR/RABINO, DAISY A..xlsx
+++ b/NEW HR/RABINO, DAISY A..xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\NEW HR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\NEW HR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E973B954-352D-44A9-BEAD-388908AA79A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -26,7 +25,7 @@
     <definedName name="BALANCE_1">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>PERIOD</t>
   </si>
@@ -187,11 +186,14 @@
   <si>
     <t>TOTAL LEAVE</t>
   </si>
+  <si>
+    <t>2024</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -567,15 +569,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -588,11 +581,20 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1048,7 +1050,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1091,7 +1093,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1155,7 +1157,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1215,7 +1217,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1281,7 +1283,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1344,7 +1346,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1442,7 +1444,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1501,7 +1503,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1566,7 +1568,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1609,7 +1611,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1684,7 +1686,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1870,7 +1872,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1936,7 +1938,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1994,7 +1996,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2060,7 +2062,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2116,7 +2118,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2191,7 +2193,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2234,7 +2236,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2300,7 +2302,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2356,7 +2358,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2454,7 +2456,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2517,7 +2519,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2566,7 +2568,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2583,25 +2585,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table15" displayName="Table15" ref="A8:K115" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A8:K116" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="16">
+    <tableColumn id="1" name="PERIOD" dataDxfId="20"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="19"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="18"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="17"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="16">
       <calculatedColumnFormula>SUM(Table15[EARNED])-SUM(Table15[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="14">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="15"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="12">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="13"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="12">
       <calculatedColumnFormula>SUM(Table15[[EARNED ]])-SUM(Table15[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="10"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="11"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2613,13 +2615,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="D2:G3" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="D2:G3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D2:G3" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="D2:G3"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DAYS"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="HOURS"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="MINUTES"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="EQUIVALENT HOURS" dataDxfId="5">
+    <tableColumn id="1" name="DAYS"/>
+    <tableColumn id="2" name="HOURS"/>
+    <tableColumn id="3" name="MINUTES"/>
+    <tableColumn id="4" name="EQUIVALENT HOURS" dataDxfId="5">
       <calculatedColumnFormula>SUMIFS(F7:F14,E7:E14,E3)+SUMIFS(D7:D66,C7:C66,F3)+D3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2628,14 +2630,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="J2:L3" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="J2:L3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="J2:L3" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="J2:L3"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="DATE STARTED" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="LEAVE EARN" dataDxfId="1">
+    <tableColumn id="1" name="DATE STARTED" dataDxfId="2"/>
+    <tableColumn id="2" name="LEAVE EARN" dataDxfId="1">
       <calculatedColumnFormula>J4-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="LEAVE EARNED" dataDxfId="0">
+    <tableColumn id="3" name="LEAVE EARNED" dataDxfId="0">
       <calculatedColumnFormula>IF($J$4=1,1.25,IF(ISBLANK($J$3),"---",1.25-VLOOKUP($K$3,$I$8:$K$37,2)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2939,7 +2941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2949,7 +2951,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2957,34 +2959,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K115"/>
+  <dimension ref="A2:K116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4788" topLeftCell="A58" activePane="bottomLeft"/>
+      <pane ySplit="4785" topLeftCell="A54" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58:C61"/>
+      <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -2996,16 +2998,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="55"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -3014,18 +3016,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="56">
+      <c r="F3" s="53">
         <v>43647</v>
       </c>
-      <c r="G3" s="50"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -3036,16 +3038,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="54"/>
+      <c r="K4" s="57"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -3053,7 +3055,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -3066,24 +3068,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52" t="s">
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -3118,7 +3120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -3127,7 +3129,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table15[EARNED])-SUM(Table15[Absence Undertime W/ Pay])</f>
-        <v>43.75</v>
+        <v>47.5</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3137,12 +3139,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table15[[EARNED ]])-SUM(Table15[Absence Undertime  W/ Pay])</f>
-        <v>58.75</v>
+        <v>67.5</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>41</v>
       </c>
@@ -3160,7 +3162,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="39">
         <v>43647</v>
       </c>
@@ -3180,9 +3182,9 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="39">
-        <v>43678</v>
+        <v>43708</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="13">
@@ -3200,9 +3202,9 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="39">
-        <v>43709</v>
+        <v>43738</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="13">
@@ -3220,9 +3222,9 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="39">
-        <v>43739</v>
+        <v>43769</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="13">
@@ -3240,9 +3242,9 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="39">
-        <v>43770</v>
+        <v>43799</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="13">
@@ -3260,9 +3262,9 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="39">
-        <v>43800</v>
+        <v>43830</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="13">
@@ -3280,7 +3282,7 @@
       <c r="J16" s="11"/>
       <c r="K16" s="20"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
         <v>42</v>
       </c>
@@ -3298,9 +3300,9 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="39">
-        <v>43831</v>
+        <v>43861</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="13">
@@ -3318,9 +3320,9 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="39">
-        <v>43862</v>
+        <v>43890</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="13">
@@ -3338,9 +3340,9 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="39">
-        <v>43891</v>
+        <v>43921</v>
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="13">
@@ -3358,9 +3360,9 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="39">
-        <v>43922</v>
+        <v>43951</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="13">
@@ -3378,9 +3380,9 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
-        <v>43952</v>
+        <v>43982</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="13">
@@ -3398,9 +3400,9 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="39">
-        <v>43983</v>
+        <v>44012</v>
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="13">
@@ -3418,9 +3420,9 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="39">
-        <v>44013</v>
+        <v>44043</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="13">
@@ -3438,9 +3440,9 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="39">
-        <v>44044</v>
+        <v>44074</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="13">
@@ -3458,9 +3460,9 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="39">
-        <v>44075</v>
+        <v>44104</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="13">
@@ -3478,9 +3480,9 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="39">
-        <v>44105</v>
+        <v>44135</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="13">
@@ -3498,9 +3500,9 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="39">
-        <v>44136</v>
+        <v>44165</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="13">
@@ -3518,9 +3520,9 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="39">
-        <v>44166</v>
+        <v>44196</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>47</v>
@@ -3542,7 +3544,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="47" t="s">
         <v>43</v>
       </c>
@@ -3560,9 +3562,9 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="39">
-        <v>44197</v>
+        <v>44227</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="13">
@@ -3580,9 +3582,9 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="39">
-        <v>44228</v>
+        <v>44255</v>
       </c>
       <c r="B32" s="20"/>
       <c r="C32" s="13">
@@ -3600,9 +3602,9 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="39">
-        <v>44256</v>
+        <v>44286</v>
       </c>
       <c r="B33" s="20"/>
       <c r="C33" s="13">
@@ -3620,9 +3622,9 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="39">
-        <v>44287</v>
+        <v>44316</v>
       </c>
       <c r="B34" s="20"/>
       <c r="C34" s="13">
@@ -3640,9 +3642,9 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="39">
-        <v>44317</v>
+        <v>44347</v>
       </c>
       <c r="B35" s="20"/>
       <c r="C35" s="13">
@@ -3660,9 +3662,9 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="39">
-        <v>44348</v>
+        <v>44377</v>
       </c>
       <c r="B36" s="20"/>
       <c r="C36" s="13">
@@ -3680,9 +3682,9 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="39">
-        <v>44378</v>
+        <v>44408</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="13">
@@ -3700,9 +3702,9 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="39">
-        <v>44409</v>
+        <v>44439</v>
       </c>
       <c r="B38" s="20"/>
       <c r="C38" s="13">
@@ -3720,9 +3722,9 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="39">
-        <v>44440</v>
+        <v>44469</v>
       </c>
       <c r="B39" s="20"/>
       <c r="C39" s="13">
@@ -3740,9 +3742,9 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="39">
-        <v>44470</v>
+        <v>44500</v>
       </c>
       <c r="B40" s="20"/>
       <c r="C40" s="13">
@@ -3760,9 +3762,9 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="39">
-        <v>44501</v>
+        <v>44530</v>
       </c>
       <c r="B41" s="20"/>
       <c r="C41" s="13">
@@ -3780,9 +3782,9 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="39">
-        <v>44531</v>
+        <v>44561</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>47</v>
@@ -3804,7 +3806,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="47" t="s">
         <v>44</v>
       </c>
@@ -3822,9 +3824,9 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="39">
-        <v>44562</v>
+        <v>44592</v>
       </c>
       <c r="B44" s="20"/>
       <c r="C44" s="13">
@@ -3842,9 +3844,9 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="39">
-        <v>44593</v>
+        <v>44620</v>
       </c>
       <c r="B45" s="20"/>
       <c r="C45" s="13">
@@ -3862,9 +3864,9 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="39">
-        <v>44621</v>
+        <v>44651</v>
       </c>
       <c r="B46" s="20"/>
       <c r="C46" s="13">
@@ -3882,9 +3884,9 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="39">
-        <v>44652</v>
+        <v>44681</v>
       </c>
       <c r="B47" s="20"/>
       <c r="C47" s="13">
@@ -3902,9 +3904,9 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="39">
-        <v>44682</v>
+        <v>44712</v>
       </c>
       <c r="B48" s="20"/>
       <c r="C48" s="13">
@@ -3922,9 +3924,9 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="39">
-        <v>44713</v>
+        <v>44742</v>
       </c>
       <c r="B49" s="20"/>
       <c r="C49" s="13">
@@ -3942,9 +3944,9 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="39">
-        <v>44743</v>
+        <v>44773</v>
       </c>
       <c r="B50" s="20"/>
       <c r="C50" s="13">
@@ -3962,9 +3964,9 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="39">
-        <v>44774</v>
+        <v>44804</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="13">
@@ -3982,9 +3984,9 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="39">
-        <v>44805</v>
+        <v>44834</v>
       </c>
       <c r="B52" s="20"/>
       <c r="C52" s="13">
@@ -4002,9 +4004,9 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="39">
-        <v>44835</v>
+        <v>44865</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="13">
@@ -4022,9 +4024,9 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="39">
-        <v>44866</v>
+        <v>44895</v>
       </c>
       <c r="B54" s="20"/>
       <c r="C54" s="13">
@@ -4042,9 +4044,9 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="39">
-        <v>44896</v>
+        <v>44926</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>47</v>
@@ -4066,7 +4068,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="47" t="s">
         <v>45</v>
       </c>
@@ -4084,9 +4086,9 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="39">
-        <v>44927</v>
+        <v>44957</v>
       </c>
       <c r="B57" s="20"/>
       <c r="C57" s="13">
@@ -4104,9 +4106,9 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="39">
-        <v>44958</v>
+        <v>44985</v>
       </c>
       <c r="B58" s="20"/>
       <c r="C58" s="13">
@@ -4124,9 +4126,9 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="39">
-        <v>44986</v>
+        <v>45016</v>
       </c>
       <c r="B59" s="20"/>
       <c r="C59" s="13">
@@ -4144,9 +4146,9 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="39">
-        <v>45017</v>
+        <v>45046</v>
       </c>
       <c r="B60" s="20"/>
       <c r="C60" s="13">
@@ -4164,9 +4166,9 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="39">
-        <v>45047</v>
+        <v>45077</v>
       </c>
       <c r="B61" s="20"/>
       <c r="C61" s="13">
@@ -4184,135 +4186,153 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="39">
-        <v>45078</v>
+        <v>45107</v>
       </c>
       <c r="B62" s="20"/>
-      <c r="C62" s="13"/>
+      <c r="C62" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D62" s="38"/>
       <c r="E62" s="9"/>
       <c r="F62" s="20"/>
-      <c r="G62" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G62" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H62" s="38"/>
       <c r="I62" s="9"/>
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="39">
-        <v>45108</v>
+        <v>45138</v>
       </c>
       <c r="B63" s="20"/>
-      <c r="C63" s="13"/>
+      <c r="C63" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D63" s="38"/>
       <c r="E63" s="9"/>
       <c r="F63" s="20"/>
-      <c r="G63" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G63" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H63" s="38"/>
       <c r="I63" s="9"/>
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="39">
-        <v>45139</v>
+        <v>45169</v>
       </c>
       <c r="B64" s="20"/>
-      <c r="C64" s="13"/>
+      <c r="C64" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D64" s="38"/>
       <c r="E64" s="9"/>
       <c r="F64" s="20"/>
-      <c r="G64" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G64" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H64" s="38"/>
       <c r="I64" s="9"/>
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="39">
-        <v>45170</v>
+        <v>45199</v>
       </c>
       <c r="B65" s="20"/>
-      <c r="C65" s="13"/>
+      <c r="C65" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D65" s="38"/>
       <c r="E65" s="9"/>
       <c r="F65" s="20"/>
-      <c r="G65" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G65" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H65" s="38"/>
       <c r="I65" s="9"/>
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="39">
-        <v>45200</v>
+        <v>45230</v>
       </c>
       <c r="B66" s="20"/>
-      <c r="C66" s="13"/>
+      <c r="C66" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D66" s="38"/>
       <c r="E66" s="9"/>
       <c r="F66" s="20"/>
-      <c r="G66" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G66" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H66" s="38"/>
       <c r="I66" s="9"/>
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="39">
-        <v>45231</v>
+        <v>45260</v>
       </c>
       <c r="B67" s="20"/>
-      <c r="C67" s="13"/>
+      <c r="C67" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D67" s="38"/>
       <c r="E67" s="9"/>
       <c r="F67" s="20"/>
-      <c r="G67" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G67" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H67" s="38"/>
       <c r="I67" s="9"/>
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="39">
-        <v>45261</v>
-      </c>
-      <c r="B68" s="20"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="38"/>
+        <v>45291</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C68" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D68" s="38">
+        <v>5</v>
+      </c>
       <c r="E68" s="9"/>
       <c r="F68" s="20"/>
-      <c r="G68" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G68" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H68" s="38"/>
       <c r="I68" s="9"/>
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A69" s="39">
-        <v>45292</v>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="47" t="s">
+        <v>50</v>
       </c>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -4328,9 +4348,9 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="39">
-        <v>45323</v>
+        <v>45322</v>
       </c>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -4346,9 +4366,9 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="39">
-        <v>45352</v>
+        <v>45351</v>
       </c>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -4364,9 +4384,9 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="39">
-        <v>45383</v>
+        <v>45382</v>
       </c>
       <c r="B72" s="20"/>
       <c r="C72" s="13"/>
@@ -4382,9 +4402,9 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="39">
-        <v>45413</v>
+        <v>45412</v>
       </c>
       <c r="B73" s="20"/>
       <c r="C73" s="13"/>
@@ -4400,9 +4420,9 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="39">
-        <v>45444</v>
+        <v>45443</v>
       </c>
       <c r="B74" s="20"/>
       <c r="C74" s="13"/>
@@ -4418,9 +4438,9 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="39">
-        <v>45474</v>
+        <v>45473</v>
       </c>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -4436,9 +4456,9 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="39">
-        <v>45505</v>
+        <v>45504</v>
       </c>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -4454,9 +4474,9 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="39">
-        <v>45536</v>
+        <v>45535</v>
       </c>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -4472,9 +4492,9 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="39">
-        <v>45566</v>
+        <v>45565</v>
       </c>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -4490,9 +4510,9 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="39">
-        <v>45597</v>
+        <v>45596</v>
       </c>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -4508,9 +4528,9 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="39">
-        <v>45627</v>
+        <v>45626</v>
       </c>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -4526,9 +4546,9 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="39">
-        <v>45658</v>
+        <v>45657</v>
       </c>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -4544,9 +4564,9 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="39">
-        <v>45689</v>
+        <v>45688</v>
       </c>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -4562,9 +4582,9 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="39">
-        <v>45717</v>
+        <v>45716</v>
       </c>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -4580,9 +4600,9 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="39">
-        <v>45748</v>
+        <v>45747</v>
       </c>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -4598,9 +4618,9 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="39">
-        <v>45778</v>
+        <v>45777</v>
       </c>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -4616,9 +4636,9 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="39">
-        <v>45809</v>
+        <v>45808</v>
       </c>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -4634,9 +4654,9 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="39">
-        <v>45839</v>
+        <v>45838</v>
       </c>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -4652,9 +4672,9 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="39">
-        <v>45870</v>
+        <v>45869</v>
       </c>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -4670,9 +4690,9 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="39">
-        <v>45901</v>
+        <v>45900</v>
       </c>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -4688,9 +4708,9 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="39">
-        <v>45931</v>
+        <v>45930</v>
       </c>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -4706,8 +4726,10 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A91" s="39"/>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="39">
+        <v>45961</v>
+      </c>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
       <c r="D91" s="38"/>
@@ -4722,7 +4744,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="39"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -4738,7 +4760,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="39"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -4754,7 +4776,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="39"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -4770,7 +4792,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="39"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -4786,7 +4808,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="39"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -4802,7 +4824,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="39"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -4818,7 +4840,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="39"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -4834,7 +4856,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="39"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -4850,7 +4872,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="39"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -4866,7 +4888,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="39"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -4882,7 +4904,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="39"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -4898,7 +4920,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="39"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -4914,7 +4936,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="39"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -4930,7 +4952,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="39"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -4946,7 +4968,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="39"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -4962,7 +4984,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="39"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -4978,7 +5000,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="39"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -4994,7 +5016,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="39"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -5010,7 +5032,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="39"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -5026,7 +5048,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="39"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -5042,7 +5064,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="39"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -5058,7 +5080,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="39"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -5074,7 +5096,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="39"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -5090,41 +5112,57 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A115" s="40"/>
-      <c r="B115" s="15"/>
-      <c r="C115" s="41"/>
-      <c r="D115" s="42"/>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" s="39"/>
+      <c r="B115" s="20"/>
+      <c r="C115" s="13"/>
+      <c r="D115" s="38"/>
       <c r="E115" s="9"/>
-      <c r="F115" s="15"/>
-      <c r="G115" s="41" t="str">
+      <c r="F115" s="20"/>
+      <c r="G115" s="13" t="str">
         <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H115" s="42"/>
+      <c r="H115" s="38"/>
       <c r="I115" s="9"/>
-      <c r="J115" s="12"/>
-      <c r="K115" s="15"/>
+      <c r="J115" s="11"/>
+      <c r="K115" s="20"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116" s="40"/>
+      <c r="B116" s="15"/>
+      <c r="C116" s="41"/>
+      <c r="D116" s="42"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="15"/>
+      <c r="G116" s="41" t="str">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H116" s="42"/>
+      <c r="I116" s="9"/>
+      <c r="J116" s="12"/>
+      <c r="K116" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5147,29 +5185,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="36" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="36" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="59" t="s">
         <v>32</v>
       </c>
@@ -5182,7 +5220,7 @@
       <c r="K1" s="60"/>
       <c r="L1" s="60"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -5211,7 +5249,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="D3"/>
@@ -5231,17 +5269,17 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -5265,10 +5303,10 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="48">
         <f>SUM('2018 LEAVE CREDITS'!E9,'2018 LEAVE CREDITS'!I9)</f>
-        <v>102.5</v>
+        <v>115</v>
       </c>
       <c r="C7" s="36">
         <v>1</v>
@@ -5296,7 +5334,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="36">
         <v>2</v>
       </c>
@@ -5322,7 +5360,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="36">
         <v>3</v>
       </c>
@@ -5348,7 +5386,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="36">
         <v>4</v>
       </c>
@@ -5374,7 +5412,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="36">
         <v>5</v>
       </c>
@@ -5400,7 +5438,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="36">
         <v>6</v>
       </c>
@@ -5426,7 +5464,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="36">
         <v>7</v>
       </c>
@@ -5452,7 +5490,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="36">
         <v>8</v>
       </c>
@@ -5478,7 +5516,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="36">
         <v>9</v>
       </c>
@@ -5498,7 +5536,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="36">
         <v>10</v>
       </c>
@@ -5518,7 +5556,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="36">
         <v>11</v>
       </c>
@@ -5538,7 +5576,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="36">
         <v>12</v>
       </c>
@@ -5559,7 +5597,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="36">
         <v>13</v>
       </c>
@@ -5580,7 +5618,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="36">
         <v>14</v>
       </c>
@@ -5601,7 +5639,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="36">
         <v>15</v>
       </c>
@@ -5622,7 +5660,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="36">
         <v>16</v>
       </c>
@@ -5643,7 +5681,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="36">
         <v>17</v>
       </c>
@@ -5664,7 +5702,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="36">
         <v>18</v>
       </c>
@@ -5685,7 +5723,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="36">
         <v>19</v>
       </c>
@@ -5706,7 +5744,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="36">
         <v>20</v>
       </c>
@@ -5727,7 +5765,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="36">
         <v>21</v>
       </c>
@@ -5748,7 +5786,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="36">
         <v>22</v>
       </c>
@@ -5769,7 +5807,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="36">
         <v>23</v>
       </c>
@@ -5790,7 +5828,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="36">
         <v>24</v>
       </c>
@@ -5811,7 +5849,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="36">
         <v>25</v>
       </c>
@@ -5832,7 +5870,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="36">
         <v>26</v>
       </c>
@@ -5853,7 +5891,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="36">
         <v>27</v>
       </c>
@@ -5874,7 +5912,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="36">
         <v>28</v>
       </c>
@@ -5895,7 +5933,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="36">
         <v>29</v>
       </c>
@@ -5916,7 +5954,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="36">
         <v>30</v>
       </c>
@@ -5937,7 +5975,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="36">
         <v>31</v>
       </c>
@@ -5958,7 +5996,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="36">
         <v>32</v>
       </c>
@@ -5967,7 +6005,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="36">
         <v>33</v>
       </c>
@@ -5976,7 +6014,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="36">
         <v>34</v>
       </c>
@@ -5985,7 +6023,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="36">
         <v>35</v>
       </c>
@@ -5994,7 +6032,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="36">
         <v>36</v>
       </c>
@@ -6003,7 +6041,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="36">
         <v>37</v>
       </c>
@@ -6012,7 +6050,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="36">
         <v>38</v>
       </c>
@@ -6021,7 +6059,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="36">
         <v>39</v>
       </c>
@@ -6030,7 +6068,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="36">
         <v>40</v>
       </c>
@@ -6039,7 +6077,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" s="36">
         <v>41</v>
       </c>
@@ -6048,7 +6086,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="36">
         <v>42</v>
       </c>
@@ -6057,7 +6095,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="36">
         <v>43</v>
       </c>
@@ -6066,7 +6104,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="36">
         <v>44</v>
       </c>
@@ -6075,7 +6113,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="36">
         <v>45</v>
       </c>
@@ -6084,7 +6122,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="36">
         <v>46</v>
       </c>
@@ -6093,7 +6131,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="36">
         <v>47</v>
       </c>
@@ -6102,7 +6140,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="36">
         <v>48</v>
       </c>
@@ -6111,7 +6149,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="36">
         <v>49</v>
       </c>
@@ -6120,7 +6158,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="36">
         <v>50</v>
       </c>
@@ -6129,7 +6167,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="36">
         <v>51</v>
       </c>
@@ -6138,7 +6176,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="36">
         <v>52</v>
       </c>
@@ -6147,7 +6185,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="36">
         <v>53</v>
       </c>
@@ -6156,7 +6194,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="36">
         <v>54</v>
       </c>
@@ -6165,7 +6203,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="36">
         <v>55</v>
       </c>
@@ -6174,7 +6212,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="36">
         <v>56</v>
       </c>
@@ -6183,7 +6221,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="36">
         <v>57</v>
       </c>
@@ -6192,7 +6230,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="36">
         <v>58</v>
       </c>
@@ -6201,7 +6239,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="36">
         <v>59</v>
       </c>
@@ -6210,7 +6248,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="36">
         <v>60</v>
       </c>
@@ -6219,7 +6257,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>